<commit_message>
more code and levels
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -530,7 +530,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="D8" s="9">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="D9" s="24">
         <f>K39</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2644,15 +2644,15 @@
       <c r="E18" s="8"/>
       <c r="F18" s="7" t="str">
         <f t="shared" ref="F18:F35" si="0">IF(J18,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G18" s="19"/>
       <c r="J18" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="2">
         <f>IF(J18=TRUE,D18,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
@@ -3138,7 +3138,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>